<commit_message>
extraction and standardization code for healthcare
</commit_message>
<xml_diff>
--- a/data/infrastructure/Supplementary table overview infra types.xlsx
+++ b/data/infrastructure/Supplementary table overview infra types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gmhcira\data\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD245E2E-05D6-44AD-8ED6-024A151D5BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085D7FF9-F0D0-49C0-BD19-C7D4CBC09789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="158">
   <si>
     <t>Key</t>
   </si>
@@ -496,7 +496,10 @@
     <t>education</t>
   </si>
   <si>
-    <t>Contains column 'amenity' and 'building' which are combined into one column. Drop original columns. Decide on reclassification.</t>
+    <t>Contains column 'amenity' and 'building' which are combined into one column. Dropped original columns. Still need to decide on reclassification.</t>
+  </si>
+  <si>
+    <t>Contains column 'amenity', 'building' and 'healthcare' which are combined into one column. Dropped original columns. Still need to decide on reclassification.</t>
   </si>
 </sst>
 </file>
@@ -812,6 +815,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -821,7 +825,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1105,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1274,7 +1277,7 @@
       <c r="C17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="78"/>
+      <c r="D17" s="75"/>
       <c r="E17" t="s">
         <v>36</v>
       </c>
@@ -1296,7 +1299,7 @@
       <c r="C18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="78"/>
+      <c r="D18" s="75"/>
       <c r="E18" t="s">
         <v>56</v>
       </c>
@@ -1310,7 +1313,7 @@
       <c r="C19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="78"/>
+      <c r="D19" s="75"/>
       <c r="E19" t="s">
         <v>56</v>
       </c>
@@ -1324,7 +1327,7 @@
       <c r="C20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="78"/>
+      <c r="D20" s="75"/>
       <c r="E20" t="s">
         <v>56</v>
       </c>
@@ -1338,7 +1341,7 @@
       <c r="C21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="78"/>
+      <c r="D21" s="75"/>
       <c r="E21" t="s">
         <v>56</v>
       </c>
@@ -1352,7 +1355,7 @@
       <c r="C22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="78"/>
+      <c r="D22" s="75"/>
       <c r="E22" t="s">
         <v>56</v>
       </c>
@@ -1366,7 +1369,7 @@
       <c r="C23" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="78"/>
+      <c r="D23" s="75"/>
       <c r="E23" t="s">
         <v>56</v>
       </c>
@@ -1382,7 +1385,7 @@
       <c r="C24" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="78"/>
+      <c r="D24" s="75"/>
       <c r="E24" t="s">
         <v>149</v>
       </c>
@@ -1424,6 +1427,13 @@
       <c r="C27" s="20" t="s">
         <v>91</v>
       </c>
+      <c r="D27" s="75"/>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="18"/>
@@ -1431,6 +1441,13 @@
       <c r="C28" s="20" t="s">
         <v>68</v>
       </c>
+      <c r="D28" s="75"/>
+      <c r="E28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="18"/>
@@ -1438,6 +1455,13 @@
       <c r="C29" s="20" t="s">
         <v>69</v>
       </c>
+      <c r="D29" s="75"/>
+      <c r="E29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="18"/>
@@ -1445,6 +1469,13 @@
       <c r="C30" s="20" t="s">
         <v>70</v>
       </c>
+      <c r="D30" s="75"/>
+      <c r="E30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="18"/>
@@ -1452,6 +1483,13 @@
       <c r="C31" s="20" t="s">
         <v>71</v>
       </c>
+      <c r="D31" s="75"/>
+      <c r="E31" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="26"/>
@@ -1459,6 +1497,13 @@
       <c r="C32" s="20" t="s">
         <v>75</v>
       </c>
+      <c r="D32" s="75"/>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="26"/>
@@ -1466,6 +1511,13 @@
       <c r="C33" s="20" t="s">
         <v>76</v>
       </c>
+      <c r="D33" s="75"/>
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="18"/>
@@ -1473,6 +1525,13 @@
       <c r="C34" s="20" t="s">
         <v>77</v>
       </c>
+      <c r="D34" s="75"/>
+      <c r="E34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="18"/>
@@ -1480,6 +1539,13 @@
       <c r="C35" s="20" t="s">
         <v>78</v>
       </c>
+      <c r="D35" s="75"/>
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="18"/>
@@ -1487,6 +1553,13 @@
       <c r="C36" s="20" t="s">
         <v>79</v>
       </c>
+      <c r="D36" s="75"/>
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="18"/>
@@ -1494,6 +1567,13 @@
       <c r="C37" s="20" t="s">
         <v>89</v>
       </c>
+      <c r="D37" s="75"/>
+      <c r="E37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="71"/>
@@ -1501,6 +1581,13 @@
       <c r="C38" s="20" t="s">
         <v>90</v>
       </c>
+      <c r="D38" s="75"/>
+      <c r="E38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="21" t="s">
@@ -1512,7 +1599,7 @@
       <c r="C39" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="78"/>
+      <c r="D39" s="75"/>
       <c r="E39" t="s">
         <v>155</v>
       </c>
@@ -1526,9 +1613,12 @@
       <c r="C40" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="78"/>
+      <c r="D40" s="75"/>
       <c r="E40" t="s">
         <v>155</v>
+      </c>
+      <c r="F40" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1537,9 +1627,12 @@
       <c r="C41" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="78"/>
+      <c r="D41" s="75"/>
       <c r="E41" t="s">
         <v>155</v>
+      </c>
+      <c r="F41" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1548,9 +1641,12 @@
       <c r="C42" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D42" s="78"/>
+      <c r="D42" s="75"/>
       <c r="E42" t="s">
         <v>155</v>
+      </c>
+      <c r="F42" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1559,9 +1655,12 @@
       <c r="C43" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="78"/>
+      <c r="D43" s="75"/>
       <c r="E43" t="s">
         <v>155</v>
+      </c>
+      <c r="F43" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2546,7 +2645,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="38"/>
-      <c r="B56" s="75" t="s">
+      <c r="B56" s="76" t="s">
         <v>59</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -2565,7 +2664,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="38"/>
-      <c r="B57" s="76"/>
+      <c r="B57" s="77"/>
       <c r="C57" s="5" t="s">
         <v>60</v>
       </c>
@@ -2582,7 +2681,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="10"/>
-      <c r="B58" s="77"/>
+      <c r="B58" s="78"/>
       <c r="C58" s="5" t="s">
         <v>60</v>
       </c>

</xml_diff>